<commit_message>
add analyse watchlist to boors func
</commit_message>
<xml_diff>
--- a/database/industries/methanol/shefan/income/quarterly/rial.xlsx
+++ b/database/industries/methanol/shefan/income/quarterly/rial.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="e:\Trade\database\industries\methanol\shefan\income\quarterly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Trade\database\industries\methanol\shefan\income\quarterly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A9DECE-2579-462A-964F-BC10C93B7328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Pouya Finance</t>
   </si>
@@ -113,9 +112,6 @@
   </si>
   <si>
     <t>هزینه کاهش ارزش دریافتنی‌‏ها (هزینه استثنایی)</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>خالص سایر درامدها (هزینه ها) ی عملیاتی</t>
@@ -157,7 +153,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -338,7 +334,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -350,7 +346,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -397,23 +393,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -449,23 +428,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -617,12 +579,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="54" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
@@ -633,7 +595,7 @@
     <col min="12" max="13" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -647,7 +609,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -663,7 +625,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -679,7 +641,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -693,7 +655,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="2:13" ht="40.799999999999997" x14ac:dyDescent="0.75">
+    <row r="5" spans="2:13" ht="42" x14ac:dyDescent="0.65">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -709,7 +671,7 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="2:13" ht="40.799999999999997" x14ac:dyDescent="0.75">
+    <row r="6" spans="2:13" ht="42" x14ac:dyDescent="0.65">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -725,7 +687,7 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -739,7 +701,7 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
@@ -775,7 +737,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>15</v>
       </c>
@@ -811,7 +773,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -825,619 +787,619 @@
       <c r="L10" s="11"/>
       <c r="M10" s="11"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13">
-        <v>0</v>
+        <v>6380553</v>
       </c>
       <c r="E11" s="13">
-        <v>0</v>
+        <v>10258553</v>
       </c>
       <c r="F11" s="13">
-        <v>0</v>
+        <v>16569944</v>
       </c>
       <c r="G11" s="13">
-        <v>0</v>
+        <v>22000891</v>
       </c>
       <c r="H11" s="13">
-        <v>0</v>
+        <v>18316084</v>
       </c>
       <c r="I11" s="13">
-        <v>0</v>
+        <v>23048931</v>
       </c>
       <c r="J11" s="13">
-        <v>0</v>
+        <v>28572723</v>
       </c>
       <c r="K11" s="13">
-        <v>0</v>
+        <v>24060951</v>
       </c>
       <c r="L11" s="13">
-        <v>0</v>
+        <v>21025634</v>
       </c>
       <c r="M11" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+        <v>24433143</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
         <v>27</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11">
-        <v>0</v>
+        <v>-3020841</v>
       </c>
       <c r="E12" s="11">
-        <v>0</v>
+        <v>-3879942</v>
       </c>
       <c r="F12" s="11">
-        <v>0</v>
+        <v>-7900097</v>
       </c>
       <c r="G12" s="11">
-        <v>0</v>
+        <v>-9019519</v>
       </c>
       <c r="H12" s="11">
-        <v>0</v>
+        <v>-5741503</v>
       </c>
       <c r="I12" s="11">
-        <v>0</v>
+        <v>-9982655</v>
       </c>
       <c r="J12" s="11">
-        <v>0</v>
+        <v>-16642468</v>
       </c>
       <c r="K12" s="11">
-        <v>0</v>
+        <v>-26432559</v>
       </c>
       <c r="L12" s="11">
-        <v>0</v>
+        <v>-14323376</v>
       </c>
       <c r="M12" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+        <v>-19801819</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
         <v>28</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15">
-        <v>0</v>
+        <v>3359712</v>
       </c>
       <c r="E13" s="15">
-        <v>0</v>
+        <v>6378611</v>
       </c>
       <c r="F13" s="15">
-        <v>0</v>
+        <v>8669847</v>
       </c>
       <c r="G13" s="15">
-        <v>0</v>
+        <v>12981372</v>
       </c>
       <c r="H13" s="15">
-        <v>0</v>
+        <v>12574581</v>
       </c>
       <c r="I13" s="15">
-        <v>0</v>
+        <v>13066276</v>
       </c>
       <c r="J13" s="15">
-        <v>0</v>
+        <v>11930255</v>
       </c>
       <c r="K13" s="15">
-        <v>0</v>
+        <v>-2371608</v>
       </c>
       <c r="L13" s="15">
-        <v>0</v>
+        <v>6702258</v>
       </c>
       <c r="M13" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+        <v>4631324</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11">
-        <v>0</v>
+        <v>-1224261</v>
       </c>
       <c r="E14" s="11">
-        <v>0</v>
+        <v>-2235395</v>
       </c>
       <c r="F14" s="11">
-        <v>0</v>
+        <v>-2425117</v>
       </c>
       <c r="G14" s="11">
-        <v>0</v>
+        <v>-2110943</v>
       </c>
       <c r="H14" s="11">
-        <v>0</v>
+        <v>-1531130</v>
       </c>
       <c r="I14" s="11">
-        <v>0</v>
+        <v>-1602051</v>
       </c>
       <c r="J14" s="11">
-        <v>0</v>
+        <v>-1410436</v>
       </c>
       <c r="K14" s="11">
-        <v>0</v>
+        <v>-1439906</v>
       </c>
       <c r="L14" s="11">
-        <v>0</v>
+        <v>-1654718</v>
       </c>
       <c r="M14" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+        <v>-2440730</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="12" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="13"/>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="13">
+        <v>0</v>
+      </c>
+      <c r="E15" s="13">
+        <v>0</v>
+      </c>
+      <c r="F15" s="13">
+        <v>0</v>
+      </c>
+      <c r="G15" s="13">
+        <v>0</v>
+      </c>
+      <c r="H15" s="13">
+        <v>0</v>
+      </c>
+      <c r="I15" s="13">
+        <v>0</v>
+      </c>
+      <c r="J15" s="13">
+        <v>0</v>
+      </c>
+      <c r="K15" s="13">
+        <v>0</v>
+      </c>
+      <c r="L15" s="13">
+        <v>0</v>
+      </c>
+      <c r="M15" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="s">
         <v>31</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I15" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="J15" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="K15" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="L15" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="M15" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="10" t="s">
-        <v>32</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11">
-        <v>0</v>
+        <v>857826</v>
       </c>
       <c r="E16" s="11">
-        <v>0</v>
+        <v>1657487</v>
       </c>
       <c r="F16" s="11">
-        <v>0</v>
+        <v>1438784</v>
       </c>
       <c r="G16" s="11">
-        <v>0</v>
+        <v>-1340575</v>
       </c>
       <c r="H16" s="11">
-        <v>0</v>
+        <v>503886</v>
       </c>
       <c r="I16" s="11">
-        <v>0</v>
+        <v>-110803</v>
       </c>
       <c r="J16" s="11">
-        <v>0</v>
+        <v>434058</v>
       </c>
       <c r="K16" s="11">
-        <v>0</v>
+        <v>-200646</v>
       </c>
       <c r="L16" s="11">
-        <v>0</v>
+        <v>749515</v>
       </c>
       <c r="M16" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+        <v>112311</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15">
-        <v>0</v>
+        <v>2993277</v>
       </c>
       <c r="E17" s="15">
-        <v>0</v>
+        <v>5800703</v>
       </c>
       <c r="F17" s="15">
-        <v>0</v>
+        <v>7683514</v>
       </c>
       <c r="G17" s="15">
-        <v>0</v>
+        <v>9529854</v>
       </c>
       <c r="H17" s="15">
-        <v>0</v>
+        <v>11547337</v>
       </c>
       <c r="I17" s="15">
-        <v>0</v>
+        <v>11353422</v>
       </c>
       <c r="J17" s="15">
-        <v>0</v>
+        <v>10953877</v>
       </c>
       <c r="K17" s="15">
-        <v>0</v>
+        <v>-4012160</v>
       </c>
       <c r="L17" s="15">
-        <v>0</v>
+        <v>5797055</v>
       </c>
       <c r="M17" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+        <v>2302905</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11">
-        <v>0</v>
+        <v>-669431</v>
       </c>
       <c r="E18" s="11">
-        <v>0</v>
+        <v>-561120</v>
       </c>
       <c r="F18" s="11">
-        <v>0</v>
+        <v>-685951</v>
       </c>
       <c r="G18" s="11">
-        <v>0</v>
+        <v>-765593</v>
       </c>
       <c r="H18" s="11">
-        <v>0</v>
+        <v>-619674</v>
       </c>
       <c r="I18" s="11">
-        <v>0</v>
+        <v>-593102</v>
       </c>
       <c r="J18" s="11">
-        <v>0</v>
+        <v>-918412</v>
       </c>
       <c r="K18" s="11">
-        <v>0</v>
+        <v>-1103609</v>
       </c>
       <c r="L18" s="11">
-        <v>0</v>
+        <v>-1310591</v>
       </c>
       <c r="M18" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+        <v>-1902898</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="13">
-        <v>0</v>
+        <v>90784</v>
       </c>
       <c r="E19" s="13">
-        <v>0</v>
+        <v>10695745</v>
       </c>
       <c r="F19" s="13">
-        <v>0</v>
+        <v>40809054</v>
       </c>
       <c r="G19" s="13">
-        <v>0</v>
+        <v>-13745178</v>
       </c>
       <c r="H19" s="13">
-        <v>0</v>
+        <v>236359</v>
       </c>
       <c r="I19" s="13">
-        <v>0</v>
+        <v>-3366694</v>
       </c>
       <c r="J19" s="13">
-        <v>0</v>
+        <v>612617</v>
       </c>
       <c r="K19" s="13">
-        <v>0</v>
+        <v>850483</v>
       </c>
       <c r="L19" s="13">
-        <v>0</v>
+        <v>1628417</v>
       </c>
       <c r="M19" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+        <v>-530347</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="17">
-        <v>0</v>
+        <v>2414630</v>
       </c>
       <c r="E20" s="17">
-        <v>0</v>
+        <v>15935328</v>
       </c>
       <c r="F20" s="17">
-        <v>0</v>
+        <v>47806617</v>
       </c>
       <c r="G20" s="17">
-        <v>0</v>
+        <v>-4980917</v>
       </c>
       <c r="H20" s="17">
-        <v>0</v>
+        <v>11164022</v>
       </c>
       <c r="I20" s="17">
-        <v>0</v>
+        <v>7393626</v>
       </c>
       <c r="J20" s="17">
-        <v>0</v>
+        <v>10648082</v>
       </c>
       <c r="K20" s="17">
-        <v>0</v>
+        <v>-4265286</v>
       </c>
       <c r="L20" s="17">
-        <v>0</v>
+        <v>6114881</v>
       </c>
       <c r="M20" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+        <v>-130340</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="13">
-        <v>0</v>
+        <v>-877</v>
       </c>
       <c r="E21" s="13">
-        <v>0</v>
+        <v>-419868</v>
       </c>
       <c r="F21" s="13">
-        <v>0</v>
+        <v>-375697</v>
       </c>
       <c r="G21" s="13">
-        <v>0</v>
-      </c>
-      <c r="H21" s="13" t="s">
-        <v>31</v>
+        <v>796442</v>
+      </c>
+      <c r="H21" s="13">
+        <v>0</v>
       </c>
       <c r="I21" s="13">
-        <v>0</v>
+        <v>-4030629</v>
       </c>
       <c r="J21" s="13">
-        <v>0</v>
+        <v>-852574</v>
       </c>
       <c r="K21" s="13">
-        <v>0</v>
+        <v>591141</v>
       </c>
       <c r="L21" s="13">
-        <v>0</v>
+        <v>-699801</v>
       </c>
       <c r="M21" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+        <v>-78143</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22" s="17"/>
       <c r="D22" s="17">
-        <v>0</v>
+        <v>2413753</v>
       </c>
       <c r="E22" s="17">
-        <v>0</v>
+        <v>15515460</v>
       </c>
       <c r="F22" s="17">
-        <v>0</v>
+        <v>47430920</v>
       </c>
       <c r="G22" s="17">
-        <v>0</v>
+        <v>-4184475</v>
       </c>
       <c r="H22" s="17">
-        <v>0</v>
+        <v>11164022</v>
       </c>
       <c r="I22" s="17">
-        <v>0</v>
+        <v>3362997</v>
       </c>
       <c r="J22" s="17">
-        <v>0</v>
+        <v>9795508</v>
       </c>
       <c r="K22" s="17">
-        <v>0</v>
+        <v>-3674145</v>
       </c>
       <c r="L22" s="17">
-        <v>0</v>
+        <v>5415080</v>
       </c>
       <c r="M22" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+        <v>-208483</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13">
+        <v>0</v>
+      </c>
+      <c r="E23" s="13">
+        <v>0</v>
+      </c>
+      <c r="F23" s="13">
+        <v>0</v>
+      </c>
+      <c r="G23" s="13">
+        <v>0</v>
+      </c>
+      <c r="H23" s="13">
+        <v>0</v>
+      </c>
+      <c r="I23" s="13">
+        <v>0</v>
+      </c>
+      <c r="J23" s="13">
+        <v>0</v>
+      </c>
+      <c r="K23" s="13">
+        <v>0</v>
+      </c>
+      <c r="L23" s="13">
+        <v>0</v>
+      </c>
+      <c r="M23" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B24" s="16" t="s">
         <v>39</v>
-      </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="H23" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I23" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="J23" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="K23" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="L23" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="M23" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="16" t="s">
-        <v>40</v>
       </c>
       <c r="C24" s="17"/>
       <c r="D24" s="17">
-        <v>0</v>
+        <v>2413753</v>
       </c>
       <c r="E24" s="17">
-        <v>0</v>
+        <v>15515460</v>
       </c>
       <c r="F24" s="17">
-        <v>0</v>
+        <v>47430920</v>
       </c>
       <c r="G24" s="17">
-        <v>0</v>
+        <v>-4184475</v>
       </c>
       <c r="H24" s="17">
-        <v>0</v>
+        <v>11164022</v>
       </c>
       <c r="I24" s="17">
-        <v>0</v>
+        <v>3362997</v>
       </c>
       <c r="J24" s="17">
-        <v>0</v>
+        <v>9795508</v>
       </c>
       <c r="K24" s="17">
-        <v>0</v>
+        <v>-3674145</v>
       </c>
       <c r="L24" s="17">
-        <v>0</v>
+        <v>5415080</v>
       </c>
       <c r="M24" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+        <v>-208483</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="13">
-        <v>0</v>
+        <v>2541</v>
       </c>
       <c r="E25" s="13">
-        <v>0</v>
+        <v>16332</v>
       </c>
       <c r="F25" s="13">
-        <v>0</v>
+        <v>49927</v>
       </c>
       <c r="G25" s="13">
-        <v>0</v>
+        <v>-4405</v>
       </c>
       <c r="H25" s="13">
-        <v>0</v>
+        <v>11752</v>
       </c>
       <c r="I25" s="13">
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="J25" s="13">
-        <v>0</v>
+        <v>316</v>
       </c>
       <c r="K25" s="13">
-        <v>0</v>
+        <v>-119</v>
       </c>
       <c r="L25" s="13">
-        <v>0</v>
+        <v>175</v>
       </c>
       <c r="M25" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11">
-        <v>0</v>
+        <v>950000</v>
       </c>
       <c r="E26" s="11">
-        <v>0</v>
+        <v>950000</v>
       </c>
       <c r="F26" s="11">
-        <v>0</v>
+        <v>950000</v>
       </c>
       <c r="G26" s="11">
-        <v>0</v>
+        <v>950000</v>
       </c>
       <c r="H26" s="11">
-        <v>0</v>
+        <v>950000</v>
       </c>
       <c r="I26" s="11">
-        <v>0</v>
+        <v>30950000</v>
       </c>
       <c r="J26" s="11">
-        <v>0</v>
+        <v>30950000</v>
       </c>
       <c r="K26" s="11">
-        <v>0</v>
+        <v>30950000</v>
       </c>
       <c r="L26" s="11">
-        <v>0</v>
+        <v>30950000</v>
       </c>
       <c r="M26" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+        <v>30950000</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="13">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="E27" s="13">
-        <v>0</v>
+        <v>501</v>
       </c>
       <c r="F27" s="13">
-        <v>0</v>
+        <v>1533</v>
       </c>
       <c r="G27" s="13">
-        <v>0</v>
+        <v>-135</v>
       </c>
       <c r="H27" s="13">
-        <v>0</v>
+        <v>361</v>
       </c>
       <c r="I27" s="13">
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="J27" s="13">
-        <v>0</v>
+        <v>316</v>
       </c>
       <c r="K27" s="13">
-        <v>0</v>
+        <v>-119</v>
       </c>
       <c r="L27" s="13">
-        <v>0</v>
+        <v>175</v>
       </c>
       <c r="M27" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>

</xml_diff>